<commit_message>
Updated Changes TIMER Driver
</commit_message>
<xml_diff>
--- a/Docs/Timers.xlsx
+++ b/Docs/Timers.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xavier.rocher\Documents\Projects\FW\stm32f446re_drivers\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA472DB9-3055-417C-84CF-EEA14A343BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D50985-0C8A-43A2-8526-06B1C640BB50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="m/0134T0Mawq/bom5zdR48YTej4NTK3OIX186wO9kzxDEHV64fDehZ+FgANqUtYqECQmww9X4e5+g8v7g3fc4g==" workbookSaltValue="VWOhZFI4xYmwAjXcAVI/Vg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{7BDEF20F-BDCC-4789-A2F0-97A656B7EA9C}"/>
+    <workbookView xWindow="46590" yWindow="4845" windowWidth="28800" windowHeight="15345" xr2:uid="{7BDEF20F-BDCC-4789-A2F0-97A656B7EA9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -217,13 +217,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -231,12 +228,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -246,11 +237,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -591,7 +588,7 @@
   <dimension ref="B3:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,26 +600,26 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="F3" s="2" t="s">
+      <c r="C3" s="8"/>
+      <c r="F3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="G3" s="8"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>16000000</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>1</v>
       </c>
     </row>
@@ -630,14 +627,14 @@
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="1">
         <f>C4/G4</f>
         <v>16000000</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>1</v>
       </c>
     </row>
@@ -645,22 +642,22 @@
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="1">
         <f>C5/G5</f>
         <v>16000000</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="8"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="1">
         <f>IF(G4=1,C6,C6*2)</f>
         <v>16000000</v>
       </c>
@@ -669,7 +666,7 @@
       <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>24</v>
       </c>
     </row>
@@ -677,7 +674,7 @@
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="1">
         <f>C11/(1+C12)</f>
         <v>640000</v>
       </c>
@@ -686,20 +683,20 @@
       <c r="B14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="7">
         <f>1/C13</f>
         <v>1.5625000000000001E-6</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="F18" s="3" t="s">
+      <c r="C18" s="8"/>
+      <c r="F18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -707,15 +704,15 @@
       <c r="B19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="1">
         <f>C13*C24/1000-1</f>
-        <v>63999</v>
-      </c>
-      <c r="F19" s="10">
+        <v>31999</v>
+      </c>
+      <c r="F19" s="1">
         <f>2^16-1</f>
         <v>65535</v>
       </c>
-      <c r="G19" s="10">
+      <c r="G19" s="1">
         <f>2^32-1</f>
         <v>4294967295</v>
       </c>
@@ -724,46 +721,46 @@
       <c r="B20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="1">
         <f>C13*C26/1000-1</f>
         <v>15999</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="1">
         <f>2^16-1</f>
         <v>65535</v>
       </c>
-      <c r="G20" s="10">
+      <c r="G20" s="1">
         <f>2^32-1</f>
         <v>4294967295</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="6"/>
+      <c r="C23" s="10"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="4">
-        <v>100</v>
+      <c r="C24" s="3">
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="4">
-        <v>25</v>
+      <c r="C25" s="3">
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="4">
         <f>C24*C25/100</f>
         <v>25</v>
       </c>
@@ -815,76 +812,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="6">
         <v>4</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="6">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="6">
         <v>8</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="6">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="6">
         <v>16</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="6">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="6">
         <v>64</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="5"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="6">
         <v>128</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="5"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="6">
         <v>256</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="5"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="A10" s="6">
         <v>512</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>